<commit_message>
Chi square tested updated
</commit_message>
<xml_diff>
--- a/SampleResultsMicrobiome.xlsx
+++ b/SampleResultsMicrobiome.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaelyn\Documents\University\University 2020-2021\thesis\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaelyn\Documents\University\University 2020-2021\thesis\MicrobiomeThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B335292C-BFC4-4913-A47F-11820A2425B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE812DB-3A81-4C8C-AD91-60C5F0C1A611}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{07B5F15C-0975-43A8-A096-442B51FDD99B}"/>
+    <workbookView xWindow="13395" yWindow="1395" windowWidth="15060" windowHeight="8325" xr2:uid="{07B5F15C-0975-43A8-A096-442B51FDD99B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="334">
   <si>
     <t>authors</t>
   </si>
@@ -1032,6 +1032,9 @@
   </si>
   <si>
     <t>Abundant phyla (Proteobacteria, Actinobacteria, and Acidobacteria are also readily dispersable). rare less dispersal. abundance considered high if &gt;5%</t>
+  </si>
+  <si>
+    <t>Agricultural</t>
   </si>
 </sst>
 </file>
@@ -1389,7 +1392,7 @@
   <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2242,7 +2245,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>144</v>
       </c>
@@ -2327,7 +2330,7 @@
         <v>25</v>
       </c>
       <c r="K18" t="s">
-        <v>150</v>
+        <v>333</v>
       </c>
       <c r="L18" t="s">
         <v>159</v>
@@ -2380,7 +2383,7 @@
         <v>165</v>
       </c>
       <c r="K19" t="s">
-        <v>150</v>
+        <v>333</v>
       </c>
       <c r="L19" t="s">
         <v>166</v>
@@ -2592,7 +2595,7 @@
         <v>197</v>
       </c>
       <c r="K23" t="s">
-        <v>150</v>
+        <v>333</v>
       </c>
       <c r="L23" t="s">
         <v>198</v>

</xml_diff>